<commit_message>
Changes as of 06/05
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC02_CDS_phs003432_Sex_Female_ExpStr-Sequencing_FileType-TXT.xlsx
+++ b/InputFiles/CDS/TC02_CDS_phs003432_Sex_Female_ExpStr-Sequencing_FileType-TXT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0507\Commons_Automation\InputFiles\CDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjany0601\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB020AC6-C8B0-4AD2-A8CB-FD41538002D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E98674E-34CF-4469-AED3-5EEB71E19E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes as of 10/28
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC02_CDS_phs003432_Sex_Female_ExpStr-Sequencing_FileType-TXT.xlsx
+++ b/InputFiles/CDS/TC02_CDS_phs003432_Sex_Female_ExpStr-Sequencing_FileType-TXT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjany0601\Commons_Automation\InputFiles\CDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0909\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E98674E-34CF-4469-AED3-5EEB71E19E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70776EE3-0403-488F-848A-3C289BECD28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -151,75 +151,6 @@
     <t>TC02_CDS_phs003432_Sex_Female_ExpStr-Sequencing_FileType-TXT_WebData.xlsx</t>
   </si>
   <si>
-    <t>WITH Filtered_Files AS (
-    SELECT DISTINCT f.file_id
-    FROM df_file f
-    JOIN df_participant sp ON f."participant.study_participant_id" = sp.study_participant_id
-    JOIN df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-    JOIN df_study s ON sp."study.phs_accession" = s.phs_accession
-    JOIN df_genomic_info gi ON gi."file.file_id" = f.file_id
-    WHERE 
-        s.phs_accession = 'phs003432'
-        AND sp.gender = 'Female'
-        AND f."experimental_strategy_and_data_subtypes" = 'Sequencing'
-        AND f.file_type = 'TXT'
-),
-File_Metadata AS (
-    SELECT 
-        f.file_id,
-        f.file_name,
-        f.file_type,
-        s.study_name,
-        s.phs_accession,
-        gi.library_strategy
-    FROM Filtered_Files ff
-    JOIN df_file f ON f.file_id = ff.file_id
-    JOIN df_participant sp ON f."participant.study_participant_id" = sp.study_participant_id
-    JOIN df_study s ON sp."study.phs_accession" = s.phs_accession
-    JOIN df_genomic_info gi ON gi."file.file_id" = f.file_id
-    GROUP BY f.file_id
-),
-File_Participants AS (
-    SELECT 
-        f.file_id,
-        sp.participant_id
-    FROM Filtered_Files ff
-    JOIN df_file f ON f.file_id = ff.file_id
-    JOIN df_participant sp ON f."participant.study_participant_id" = sp.study_participant_id
-),
-File_Samples AS (
-    SELECT 
-        f.file_id,
-        smp.sample_id,
-        smp.sample_type,
-        smp.sample_tumor_status,
-        smp.sample_id || ' : ' || smp.sample_type AS sample_display
-    FROM Filtered_Files ff
-    JOIN df_file f ON f.file_id = ff.file_id
-    JOIN df_sample smp ON smp."participant.study_participant_id" = f."participant.study_participant_id"
-)
-SELECT 
-    fm.file_name AS "File Name",
-    fm.study_name AS "Study Name",
-    fm.phs_accession AS "Accession",
-    -- First 5 participant IDs
-    (SELECT GROUP_CONCAT(participant_id, ', ') 
-     FROM (SELECT participant_id FROM File_Participants WHERE file_id = fm.file_id LIMIT 5)) 
-     || CASE WHEN (SELECT COUNT(*) FROM File_Participants WHERE file_id = fm.file_id) &gt; 5 THEN ', ...' ELSE '' END 
-     AS "Participant ID",
-    -- First 5 Sample display values
-    (SELECT GROUP_CONCAT(sample_display, ', ') 
-     FROM (SELECT sample_display FROM File_Samples WHERE file_id = fm.file_id LIMIT 5)) 
-     || CASE WHEN (SELECT COUNT(*) FROM File_Samples WHERE file_id = fm.file_id) &gt; 5 THEN ', ...' ELSE '' END 
-     AS "Sample Id",
-    fm.file_type AS "File Type",
-    fm.library_strategy AS "Library Strategy",
-    '' AS "Supplementary Files"
-FROM File_Metadata fm
-ORDER BY fm.file_name
---LIMIT 100;</t>
-  </si>
-  <si>
     <t>WITH Filtered_Files AS ( 
     SELECT DISTINCT f.file_id, f."participant.study_participant_id"
     FROM df_file f
@@ -257,6 +188,137 @@
 JOIN Matched_Participants mp ON ff."participant.study_participant_id" = mp.study_participant_id
 JOIN Matched_Samples smp ON smp."participant.study_participant_id" = mp.study_participant_id
 JOIN Matched_Studies ms ON mp."study.phs_accession" = ms.phs_accession;</t>
+  </si>
+  <si>
+    <t>WITH
+  participant AS (
+    SELECT
+      study_participant_id,
+      participant_id,
+      gender,
+      "study.phs_accession" AS study_phs_accession
+    FROM df_participant
+  ),
+  study AS (
+    SELECT
+      phs_accession,
+      study_name,
+      "program.program_acronym" AS program_program_acronym
+    FROM df_study
+  ),
+  sample AS (
+    SELECT
+      sample_id,
+      "participant.study_participant_id" AS participant_study_participant_id,
+      sample_type,
+      sample_tumor_status,
+      sample_anatomic_site
+    FROM df_sample
+  ),
+  file AS (
+    SELECT
+      file_id,
+      file_name,
+      file_type,
+      "sample.sample_id" AS sample_sample_id,
+      experimental_strategy_and_data_subtypes
+    FROM df_file
+  ),
+  genomic AS (
+    SELECT
+      "file.file_id" AS file_file_id,
+      library_strategy
+    FROM df_genomic_info
+  ),
+  Filtered_Files AS (
+    SELECT DISTINCT f.file_id
+    FROM file f
+    JOIN sample smp
+      ON f.sample_sample_id = smp.sample_id
+    JOIN participant sp
+      ON smp.participant_study_participant_id = sp.study_participant_id
+    JOIN study s
+      ON sp.study_phs_accession = s.phs_accession
+    JOIN genomic gi
+      ON gi.file_file_id = f.file_id
+    WHERE
+      s.phs_accession = 'phs003432'
+      AND sp.gender = 'Female'
+      AND f.experimental_strategy_and_data_subtypes = 'Sequencing'
+      AND f.file_type = 'TXT'
+  ),
+  File_Metadata AS (
+    SELECT
+      f.file_id,
+      f.file_name,
+      f.file_type,
+      s.study_name,
+      s.phs_accession,
+      gi.library_strategy
+    FROM Filtered_Files ff
+    JOIN file f        ON f.file_id = ff.file_id
+    JOIN sample smp    ON f.sample_sample_id = smp.sample_id
+    JOIN participant sp ON smp.participant_study_participant_id = sp.study_participant_id
+    JOIN study s       ON sp.study_phs_accession = s.phs_accession
+    JOIN genomic gi    ON gi.file_file_id = f.file_id
+    GROUP BY f.file_id
+  ),
+  File_Participants AS (
+    SELECT
+      f.file_id,
+      sp.participant_id
+    FROM Filtered_Files ff
+    JOIN file f      ON f.file_id = ff.file_id
+    JOIN sample smp  ON f.sample_sample_id = smp.sample_id
+    JOIN participant sp ON smp.participant_study_participant_id = sp.study_participant_id
+  ),
+  File_Samples AS (
+    SELECT
+      f.file_id,
+      smp.sample_id,
+      smp.sample_type,
+      smp.sample_tumor_status,
+      smp.sample_anatomic_site,
+      smp.sample_id || ' : ' ||
+        COALESCE(NULLIF(TRIM(smp.sample_anatomic_site), ''), smp.sample_type) AS sample_display
+    FROM Filtered_Files ff
+    JOIN file f     ON f.file_id = ff.file_id
+    JOIN sample smp ON f.sample_sample_id = smp.sample_id
+  )
+SELECT
+  fm.file_name       AS "File Name",
+  fm.study_name      AS "Study Name",
+  fm.phs_accession   AS "Accession",
+  -- first 5 participants, with ellipsis if more
+  (
+    SELECT GROUP_CONCAT(participant_id, ', ')
+    FROM (SELECT participant_id
+          FROM File_Participants
+          WHERE file_id = fm.file_id
+          LIMIT 5)
+  )
+  || CASE
+       WHEN (SELECT COUNT(*) FROM File_Participants WHERE file_id = fm.file_id) &gt; 5
+       THEN ', ...' ELSE '' END
+  AS "Participant ID",
+  -- first 5 samples, with ellipsis if more (no duplicate site text)
+  (
+    SELECT GROUP_CONCAT(sample_display, ', ')
+    FROM (SELECT sample_display
+          FROM File_Samples
+          WHERE file_id = fm.file_id
+          LIMIT 5)
+  )
+  || CASE
+       WHEN (SELECT COUNT(*) FROM File_Samples WHERE file_id = fm.file_id) &gt; 5
+       THEN ', ...' ELSE '' END
+  AS "Sample Id",
+  fm.file_type         AS "File Type",
+  fm.library_strategy  AS "Library Strategy",
+  ''                   AS "Supplementary Files"
+FROM File_Metadata fm
+ORDER BY fm.file_name
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
@@ -648,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +747,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -708,7 +770,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>

</xml_diff>